<commit_message>
Gestion du cas Paiement par cleanway
</commit_message>
<xml_diff>
--- a/App_pressing_Loreau/Resources/PatternFile/LecturePattern.xlsx
+++ b/App_pressing_Loreau/Resources/PatternFile/LecturePattern.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>LE LOREAU 28130 Hanches</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>Chiffre d'affaire</t>
-  </si>
-  <si>
-    <t>&lt;Departement&gt;</t>
   </si>
   <si>
     <t>&lt;TTC&gt;</t>
@@ -65,11 +62,17 @@
   <si>
     <t xml:space="preserve">Nouveaux clients : </t>
   </si>
+  <si>
+    <t>Payement CleanWay</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -109,7 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -303,21 +306,6 @@
         <color theme="0"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
         <color theme="0"/>
       </top>
       <bottom style="thin">
@@ -522,21 +510,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="dotted">
         <color auto="1"/>
       </left>
@@ -553,19 +526,6 @@
       </left>
       <right style="thin">
         <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
       </right>
       <top style="thin">
         <color theme="0"/>
@@ -646,6 +606,77 @@
       </top>
       <bottom style="thin">
         <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -653,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -662,48 +693,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -713,50 +786,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1054,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1121,320 +1166,243 @@
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" ht="26.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="44"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="56"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32" t="s">
-        <v>7</v>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29" t="s">
+        <v>6</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="37" t="s">
-        <v>7</v>
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="34" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="39"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="41"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="41"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="41"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="41"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="41"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="41"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="41"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="41"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="41"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="59"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="39" t="s">
-        <v>10</v>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="41"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="46" t="s">
+        <v>15</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>6</v>
+      <c r="I20" s="47"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37" t="s">
+        <v>9</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="13"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="45" t="s">
+      <c r="L20" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="48"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="47"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="46"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="8"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="22"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="53"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" s="53"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L22" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="6"/>
@@ -1454,73 +1422,73 @@
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="51" t="s">
-        <v>8</v>
+      <c r="D24" s="50" t="s">
+        <v>7</v>
       </c>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="54" t="s">
-        <v>13</v>
+      <c r="A25" s="52" t="s">
+        <v>12</v>
       </c>
-      <c r="B25" s="55"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29" t="s">
+      <c r="B25" s="53"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="33"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="49"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="12"/>
       <c r="D26" s="17"/>
       <c r="E26" s="15"/>
       <c r="F26" s="14"/>
       <c r="G26" s="15"/>
-      <c r="H26" s="56" t="s">
-        <v>14</v>
+      <c r="H26" s="43" t="s">
+        <v>13</v>
       </c>
-      <c r="I26" s="57"/>
-      <c r="J26" s="58"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="45"/>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="7"/>
       <c r="D27" s="16"/>
       <c r="E27" s="10"/>
       <c r="F27" s="9"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="56" t="s">
-        <v>15</v>
+      <c r="H27" s="43" t="s">
+        <v>14</v>
       </c>
-      <c r="I27" s="57"/>
-      <c r="J27" s="58"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="45"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="49"/>
-      <c r="B28" s="50"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="7"/>
       <c r="D28" s="16"/>
       <c r="E28" s="10"/>
@@ -1530,204 +1498,204 @@
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="7"/>
       <c r="D29" s="16"/>
       <c r="E29" s="10"/>
       <c r="F29" s="9"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="58"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="45"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="49"/>
-      <c r="B30" s="50"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="7"/>
       <c r="D30" s="16"/>
       <c r="E30" s="10"/>
       <c r="F30" s="9"/>
       <c r="G30" s="10"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="58"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="45"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="49"/>
-      <c r="B31" s="50"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="7"/>
       <c r="D31" s="16"/>
       <c r="E31" s="10"/>
       <c r="F31" s="9"/>
       <c r="G31" s="10"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="58"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="45"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="49"/>
-      <c r="B32" s="50"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="40"/>
       <c r="C32" s="7"/>
       <c r="D32" s="16"/>
       <c r="E32" s="10"/>
       <c r="F32" s="9"/>
       <c r="G32" s="10"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="57"/>
-      <c r="J32" s="58"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="45"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="49"/>
-      <c r="B33" s="50"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="7"/>
       <c r="D33" s="16"/>
       <c r="E33" s="10"/>
       <c r="F33" s="9"/>
       <c r="G33" s="10"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="57"/>
-      <c r="J33" s="58"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="45"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="49"/>
-      <c r="B34" s="50"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="40"/>
       <c r="C34" s="7"/>
       <c r="D34" s="16"/>
       <c r="E34" s="10"/>
       <c r="F34" s="9"/>
       <c r="G34" s="10"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="58"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="45"/>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="49"/>
-      <c r="B35" s="50"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="40"/>
       <c r="C35" s="7"/>
       <c r="D35" s="16"/>
       <c r="E35" s="10"/>
       <c r="F35" s="9"/>
       <c r="G35" s="10"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="58"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="45"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="49"/>
-      <c r="B36" s="50"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="7"/>
       <c r="D36" s="16"/>
       <c r="E36" s="10"/>
       <c r="F36" s="9"/>
       <c r="G36" s="10"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="58"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="45"/>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="49"/>
-      <c r="B37" s="50"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="18"/>
       <c r="D37" s="16"/>
       <c r="E37" s="19"/>
       <c r="F37" s="9"/>
       <c r="G37" s="10"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="57"/>
-      <c r="J37" s="58"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="45"/>
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="49"/>
-      <c r="B38" s="50"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="7"/>
       <c r="D38" s="16"/>
       <c r="E38" s="10"/>
       <c r="F38" s="9"/>
       <c r="G38" s="10"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="58"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="45"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="49"/>
-      <c r="B39" s="50"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="7"/>
       <c r="D39" s="16"/>
       <c r="E39" s="10"/>
       <c r="F39" s="9"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="57"/>
-      <c r="J39" s="58"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="45"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="49"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="40"/>
       <c r="C40" s="7"/>
       <c r="D40" s="16"/>
       <c r="E40" s="10"/>
       <c r="F40" s="9"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="57"/>
-      <c r="J40" s="58"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="45"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="49"/>
-      <c r="B41" s="50"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="40"/>
       <c r="C41" s="7"/>
       <c r="D41" s="16"/>
       <c r="E41" s="10"/>
       <c r="F41" s="9"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="57"/>
-      <c r="J41" s="58"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="45"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="49"/>
-      <c r="B42" s="50"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="40"/>
       <c r="C42" s="7"/>
       <c r="D42" s="16"/>
       <c r="E42" s="10"/>
       <c r="F42" s="9"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="56"/>
-      <c r="I42" s="57"/>
-      <c r="J42" s="58"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="45"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="49"/>
-      <c r="B43" s="50"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="7"/>
       <c r="D43" s="16"/>
       <c r="E43" s="10"/>
@@ -1740,8 +1708,8 @@
       <c r="L43" s="6"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="49"/>
-      <c r="B44" s="50"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="18"/>
       <c r="D44" s="16"/>
       <c r="E44" s="19"/>
@@ -1768,8 +1736,8 @@
       <c r="L45" s="6"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="45"/>
-      <c r="B46" s="59"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="42"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -2160,7 +2128,55 @@
       <c r="L73" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="66">
+  <mergeCells count="64">
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="H26:J26"/>
@@ -2177,56 +2193,6 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H37:J37"/>
     <mergeCell ref="H38:J38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Deuxieme modification depuis modif bdd. Avant test général de la modif
</commit_message>
<xml_diff>
--- a/App_pressing_Loreau/Resources/PatternFile/LecturePattern.xlsx
+++ b/App_pressing_Loreau/Resources/PatternFile/LecturePattern.xlsx
@@ -684,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -734,66 +734,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -805,6 +745,72 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1100,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:L73"/>
+  <dimension ref="A2:L155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1169,33 +1175,33 @@
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" ht="26.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="41"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="66"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -1219,190 +1225,190 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="53"/>
-      <c r="B10" s="54"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="11"/>
       <c r="D10" s="33"/>
-      <c r="E10" s="59"/>
+      <c r="E10" s="39"/>
       <c r="F10" s="12"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="54"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="48"/>
       <c r="J10" s="11"/>
       <c r="K10" s="33"/>
-      <c r="L10" s="63"/>
+      <c r="L10" s="43"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="42"/>
-      <c r="B11" s="43"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="7"/>
       <c r="D11" s="34"/>
-      <c r="E11" s="60"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="54"/>
       <c r="J11" s="7"/>
       <c r="K11" s="34"/>
-      <c r="L11" s="64"/>
+      <c r="L11" s="44"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="42"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="7"/>
       <c r="D12" s="34"/>
-      <c r="E12" s="60"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="43"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="54"/>
       <c r="J12" s="7"/>
       <c r="K12" s="34"/>
-      <c r="L12" s="64"/>
+      <c r="L12" s="44"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="42"/>
-      <c r="B13" s="43"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="7"/>
       <c r="D13" s="34"/>
-      <c r="E13" s="60"/>
+      <c r="E13" s="40"/>
       <c r="F13" s="8"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="43"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="54"/>
       <c r="J13" s="7"/>
       <c r="K13" s="34"/>
-      <c r="L13" s="64"/>
+      <c r="L13" s="44"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="42"/>
-      <c r="B14" s="43"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="7"/>
       <c r="D14" s="34"/>
-      <c r="E14" s="60"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="8"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="43"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
       <c r="J14" s="7"/>
       <c r="K14" s="34"/>
-      <c r="L14" s="64"/>
+      <c r="L14" s="44"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="42"/>
-      <c r="B15" s="43"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="7"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="60"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="8"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="43"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="54"/>
       <c r="J15" s="7"/>
       <c r="K15" s="34"/>
-      <c r="L15" s="64"/>
+      <c r="L15" s="44"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="42"/>
-      <c r="B16" s="43"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="7"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="60"/>
+      <c r="E16" s="40"/>
       <c r="F16" s="8"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="43"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="54"/>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
-      <c r="L16" s="64"/>
+      <c r="L16" s="44"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="42"/>
-      <c r="B17" s="43"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="7"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="60"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="43"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="54"/>
       <c r="J17" s="7"/>
       <c r="K17" s="34"/>
-      <c r="L17" s="64"/>
+      <c r="L17" s="44"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="42"/>
-      <c r="B18" s="43"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="7"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="60"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="8"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="54"/>
       <c r="J18" s="7"/>
       <c r="K18" s="34"/>
-      <c r="L18" s="64"/>
+      <c r="L18" s="44"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="42"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="7"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="60"/>
+      <c r="E19" s="40"/>
       <c r="F19" s="8"/>
       <c r="G19" s="36"/>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="45"/>
+      <c r="I19" s="58"/>
       <c r="J19" s="37"/>
       <c r="K19" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="L19" s="65" t="s">
+      <c r="L19" s="45" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="42"/>
-      <c r="B20" s="43"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="7"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="60"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="8"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="49" t="s">
+      <c r="H20" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="50"/>
+      <c r="I20" s="56"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="66">
+      <c r="L20" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="51"/>
-      <c r="B21" s="52"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="63"/>
       <c r="C21" s="16"/>
       <c r="D21" s="35"/>
-      <c r="E21" s="61"/>
+      <c r="E21" s="41"/>
       <c r="F21" s="18"/>
       <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="50"/>
+      <c r="B22" s="56"/>
       <c r="C22" s="20"/>
       <c r="D22" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="62" t="s">
+      <c r="E22" s="42" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="21"/>
@@ -1425,23 +1431,23 @@
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="47"/>
+      <c r="B25" s="60"/>
       <c r="C25" s="23"/>
       <c r="D25" s="23" t="s">
         <v>10</v>
@@ -1458,40 +1464,40 @@
       <c r="L25" s="23"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="53"/>
-      <c r="B26" s="54"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="48"/>
       <c r="C26" s="11"/>
       <c r="D26" s="15"/>
       <c r="E26" s="13"/>
       <c r="F26" s="12"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="55" t="s">
+      <c r="H26" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="56"/>
-      <c r="J26" s="57"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="53"/>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="53"/>
-      <c r="B27" s="54"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="48"/>
       <c r="C27" s="7"/>
       <c r="D27" s="14"/>
       <c r="E27" s="9"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="55" t="s">
+      <c r="H27" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="56"/>
-      <c r="J27" s="57"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="53"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="53"/>
-      <c r="B28" s="54"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="7"/>
       <c r="D28" s="14"/>
       <c r="E28" s="9"/>
@@ -1501,204 +1507,204 @@
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="53"/>
-      <c r="B29" s="54"/>
+      <c r="A29" s="47"/>
+      <c r="B29" s="48"/>
       <c r="C29" s="7"/>
       <c r="D29" s="14"/>
       <c r="E29" s="9"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="57"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="53"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="53"/>
-      <c r="B30" s="54"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="48"/>
       <c r="C30" s="7"/>
       <c r="D30" s="14"/>
       <c r="E30" s="9"/>
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="57"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="53"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="53"/>
-      <c r="B31" s="54"/>
+      <c r="A31" s="47"/>
+      <c r="B31" s="48"/>
       <c r="C31" s="7"/>
       <c r="D31" s="14"/>
       <c r="E31" s="9"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="57"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="53"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="53"/>
-      <c r="B32" s="54"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="48"/>
       <c r="C32" s="7"/>
       <c r="D32" s="14"/>
       <c r="E32" s="9"/>
       <c r="F32" s="8"/>
       <c r="G32" s="9"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="57"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="53"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="53"/>
-      <c r="B33" s="54"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="48"/>
       <c r="C33" s="7"/>
       <c r="D33" s="14"/>
       <c r="E33" s="9"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="57"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="53"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="53"/>
-      <c r="B34" s="54"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="48"/>
       <c r="C34" s="7"/>
       <c r="D34" s="14"/>
       <c r="E34" s="9"/>
       <c r="F34" s="8"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="57"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="53"/>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="53"/>
-      <c r="B35" s="54"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="48"/>
       <c r="C35" s="7"/>
       <c r="D35" s="14"/>
       <c r="E35" s="9"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="57"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="53"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="53"/>
-      <c r="B36" s="54"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="7"/>
       <c r="D36" s="14"/>
       <c r="E36" s="9"/>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="57"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="53"/>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="53"/>
-      <c r="B37" s="54"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="48"/>
       <c r="C37" s="16"/>
       <c r="D37" s="14"/>
       <c r="E37" s="17"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="57"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="53"/>
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="53"/>
-      <c r="B38" s="54"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="48"/>
       <c r="C38" s="7"/>
       <c r="D38" s="14"/>
       <c r="E38" s="9"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="57"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="53"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="53"/>
-      <c r="B39" s="54"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="48"/>
       <c r="C39" s="7"/>
       <c r="D39" s="14"/>
       <c r="E39" s="9"/>
       <c r="F39" s="8"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="57"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="53"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="53"/>
-      <c r="B40" s="54"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="48"/>
       <c r="C40" s="7"/>
       <c r="D40" s="14"/>
       <c r="E40" s="9"/>
       <c r="F40" s="8"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="56"/>
-      <c r="J40" s="57"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="53"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="53"/>
-      <c r="B41" s="54"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="48"/>
       <c r="C41" s="7"/>
       <c r="D41" s="14"/>
       <c r="E41" s="9"/>
       <c r="F41" s="8"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="56"/>
-      <c r="J41" s="57"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="53"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="53"/>
-      <c r="B42" s="54"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="14"/>
       <c r="E42" s="9"/>
       <c r="F42" s="8"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="56"/>
-      <c r="J42" s="57"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="53"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="53"/>
-      <c r="B43" s="54"/>
+      <c r="A43" s="47"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="7"/>
       <c r="D43" s="14"/>
       <c r="E43" s="9"/>
@@ -1711,8 +1717,8 @@
       <c r="L43" s="6"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="53"/>
-      <c r="B44" s="54"/>
+      <c r="A44" s="47"/>
+      <c r="B44" s="48"/>
       <c r="C44" s="16"/>
       <c r="D44" s="14"/>
       <c r="E44" s="17"/>
@@ -1725,8 +1731,8 @@
       <c r="L44" s="6"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
+      <c r="A45" s="67"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -1739,8 +1745,8 @@
       <c r="L45" s="6"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="42"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="50"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -1753,8 +1759,8 @@
       <c r="L46" s="6"/>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
+      <c r="A47" s="67"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -1767,8 +1773,8 @@
       <c r="L47" s="6"/>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
+      <c r="A48" s="67"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -1781,8 +1787,8 @@
       <c r="L48" s="6"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
+      <c r="A49" s="67"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -1795,8 +1801,8 @@
       <c r="L49" s="6"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
+      <c r="A50" s="67"/>
+      <c r="B50" s="67"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
@@ -1809,8 +1815,8 @@
       <c r="L50" s="6"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
+      <c r="A51" s="67"/>
+      <c r="B51" s="67"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -1823,8 +1829,8 @@
       <c r="L51" s="6"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
+      <c r="A52" s="67"/>
+      <c r="B52" s="67"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -1837,8 +1843,8 @@
       <c r="L52" s="6"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
+      <c r="A53" s="67"/>
+      <c r="B53" s="67"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -1851,8 +1857,8 @@
       <c r="L53" s="6"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
+      <c r="A54" s="67"/>
+      <c r="B54" s="67"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -1865,8 +1871,8 @@
       <c r="L54" s="6"/>
     </row>
     <row r="55" spans="1:12">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
+      <c r="A55" s="67"/>
+      <c r="B55" s="67"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -1879,8 +1885,8 @@
       <c r="L55" s="6"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
+      <c r="A56" s="67"/>
+      <c r="B56" s="67"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -1893,8 +1899,8 @@
       <c r="L56" s="6"/>
     </row>
     <row r="57" spans="1:12">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
+      <c r="A57" s="67"/>
+      <c r="B57" s="67"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -1907,8 +1913,8 @@
       <c r="L57" s="6"/>
     </row>
     <row r="58" spans="1:12">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
+      <c r="A58" s="67"/>
+      <c r="B58" s="67"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
@@ -1921,8 +1927,8 @@
       <c r="L58" s="6"/>
     </row>
     <row r="59" spans="1:12">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6"/>
+      <c r="A59" s="67"/>
+      <c r="B59" s="67"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
@@ -1935,8 +1941,8 @@
       <c r="L59" s="6"/>
     </row>
     <row r="60" spans="1:12">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6"/>
+      <c r="A60" s="67"/>
+      <c r="B60" s="67"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
@@ -1949,8 +1955,8 @@
       <c r="L60" s="6"/>
     </row>
     <row r="61" spans="1:12">
-      <c r="A61" s="6"/>
-      <c r="B61" s="6"/>
+      <c r="A61" s="67"/>
+      <c r="B61" s="67"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
@@ -1963,8 +1969,8 @@
       <c r="L61" s="6"/>
     </row>
     <row r="62" spans="1:12">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
+      <c r="A62" s="67"/>
+      <c r="B62" s="67"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
@@ -1977,8 +1983,8 @@
       <c r="L62" s="6"/>
     </row>
     <row r="63" spans="1:12">
-      <c r="A63" s="6"/>
-      <c r="B63" s="6"/>
+      <c r="A63" s="67"/>
+      <c r="B63" s="67"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
@@ -1991,8 +1997,8 @@
       <c r="L63" s="6"/>
     </row>
     <row r="64" spans="1:12">
-      <c r="A64" s="6"/>
-      <c r="B64" s="6"/>
+      <c r="A64" s="67"/>
+      <c r="B64" s="67"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
@@ -2005,8 +2011,8 @@
       <c r="L64" s="6"/>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="6"/>
-      <c r="B65" s="6"/>
+      <c r="A65" s="67"/>
+      <c r="B65" s="67"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
@@ -2019,8 +2025,8 @@
       <c r="L65" s="6"/>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6"/>
+      <c r="A66" s="67"/>
+      <c r="B66" s="67"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
@@ -2033,8 +2039,8 @@
       <c r="L66" s="6"/>
     </row>
     <row r="67" spans="1:12">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6"/>
+      <c r="A67" s="67"/>
+      <c r="B67" s="67"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
@@ -2047,8 +2053,8 @@
       <c r="L67" s="6"/>
     </row>
     <row r="68" spans="1:12">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6"/>
+      <c r="A68" s="67"/>
+      <c r="B68" s="67"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
@@ -2061,8 +2067,8 @@
       <c r="L68" s="6"/>
     </row>
     <row r="69" spans="1:12">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6"/>
+      <c r="A69" s="67"/>
+      <c r="B69" s="67"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
@@ -2075,8 +2081,8 @@
       <c r="L69" s="6"/>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6"/>
+      <c r="A70" s="67"/>
+      <c r="B70" s="67"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
@@ -2089,8 +2095,8 @@
       <c r="L70" s="6"/>
     </row>
     <row r="71" spans="1:12">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
+      <c r="A71" s="67"/>
+      <c r="B71" s="67"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
@@ -2103,8 +2109,8 @@
       <c r="L71" s="6"/>
     </row>
     <row r="72" spans="1:12">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
+      <c r="A72" s="67"/>
+      <c r="B72" s="67"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
@@ -2117,8 +2123,8 @@
       <c r="L72" s="6"/>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
+      <c r="A73" s="67"/>
+      <c r="B73" s="67"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
@@ -2130,8 +2136,384 @@
       <c r="K73" s="6"/>
       <c r="L73" s="6"/>
     </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="68"/>
+      <c r="B74" s="68"/>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="68"/>
+      <c r="B75" s="68"/>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" s="68"/>
+      <c r="B76" s="68"/>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" s="68"/>
+      <c r="B77" s="68"/>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" s="68"/>
+      <c r="B78" s="68"/>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" s="68"/>
+      <c r="B79" s="68"/>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" s="68"/>
+      <c r="B80" s="68"/>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="68"/>
+      <c r="B81" s="68"/>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="68"/>
+      <c r="B82" s="68"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="68"/>
+      <c r="B83" s="68"/>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="68"/>
+      <c r="B84" s="68"/>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="68"/>
+      <c r="B85" s="68"/>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="68"/>
+      <c r="B86" s="68"/>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="68"/>
+      <c r="B87" s="68"/>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="68"/>
+      <c r="B88" s="68"/>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="68"/>
+      <c r="B89" s="68"/>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="68"/>
+      <c r="B90" s="68"/>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="68"/>
+      <c r="B91" s="68"/>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="68"/>
+      <c r="B92" s="68"/>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="68"/>
+      <c r="B93" s="68"/>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="68"/>
+      <c r="B94" s="68"/>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="68"/>
+      <c r="B95" s="68"/>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="68"/>
+      <c r="B96" s="68"/>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="68"/>
+      <c r="B97" s="68"/>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="68"/>
+      <c r="B98" s="68"/>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="68"/>
+      <c r="B99" s="68"/>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="68"/>
+      <c r="B100" s="68"/>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="68"/>
+      <c r="B101" s="68"/>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="68"/>
+      <c r="B102" s="68"/>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="68"/>
+      <c r="B103" s="68"/>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="68"/>
+      <c r="B104" s="68"/>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="68"/>
+      <c r="B105" s="68"/>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="68"/>
+      <c r="B106" s="68"/>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="68"/>
+      <c r="B107" s="68"/>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="68"/>
+      <c r="B108" s="68"/>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="68"/>
+      <c r="B109" s="68"/>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="68"/>
+      <c r="B110" s="68"/>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="68"/>
+      <c r="B111" s="68"/>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="68"/>
+      <c r="B112" s="68"/>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="68"/>
+      <c r="B113" s="68"/>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="68"/>
+      <c r="B114" s="68"/>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="68"/>
+      <c r="B115" s="68"/>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="68"/>
+      <c r="B116" s="68"/>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="68"/>
+      <c r="B117" s="68"/>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="68"/>
+      <c r="B118" s="68"/>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="68"/>
+      <c r="B119" s="68"/>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="68"/>
+      <c r="B120" s="68"/>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="68"/>
+      <c r="B121" s="68"/>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="68"/>
+      <c r="B122" s="68"/>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="68"/>
+      <c r="B123" s="68"/>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="68"/>
+      <c r="B124" s="68"/>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="68"/>
+      <c r="B125" s="68"/>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="68"/>
+      <c r="B126" s="68"/>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="68"/>
+      <c r="B127" s="68"/>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="68"/>
+      <c r="B128" s="68"/>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="68"/>
+      <c r="B129" s="68"/>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="68"/>
+      <c r="B130" s="68"/>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="68"/>
+      <c r="B131" s="68"/>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="68"/>
+      <c r="B132" s="68"/>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="68"/>
+      <c r="B133" s="68"/>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="68"/>
+      <c r="B134" s="68"/>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="68"/>
+      <c r="B135" s="68"/>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="68"/>
+      <c r="B136" s="68"/>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="68"/>
+      <c r="B137" s="68"/>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="68"/>
+      <c r="B138" s="68"/>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="68"/>
+      <c r="B139" s="68"/>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="68"/>
+      <c r="B140" s="68"/>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="68"/>
+      <c r="B141" s="68"/>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="68"/>
+      <c r="B142" s="68"/>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="68"/>
+      <c r="B143" s="68"/>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="68"/>
+      <c r="B144" s="68"/>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="68"/>
+      <c r="B145" s="68"/>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="68"/>
+      <c r="B146" s="68"/>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="68"/>
+      <c r="B147" s="68"/>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="68"/>
+      <c r="B148" s="68"/>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="68"/>
+      <c r="B149" s="68"/>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="68"/>
+      <c r="B150" s="68"/>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="68"/>
+      <c r="B151" s="68"/>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="68"/>
+      <c r="B152" s="68"/>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="68"/>
+      <c r="B153" s="68"/>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="68"/>
+      <c r="B154" s="68"/>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="68"/>
+      <c r="B155" s="68"/>
+    </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="H26:J26"/>
@@ -2148,54 +2530,6 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H37:J37"/>
     <mergeCell ref="H38:J38"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>